<commit_message>
adding test case file
</commit_message>
<xml_diff>
--- a/Test Case/nopCommerce_Test_cases.xlsx
+++ b/Test Case/nopCommerce_Test_cases.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Manual testing learning\Noo Commerce\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\manual testing\nopCommerce-Manual-Testing-Project\Test Case\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82D27AF7-5829-44B8-BB3B-0C439471D809}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14CB81E7-4AB7-481F-A754-D77AEA78B05A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="786" xr2:uid="{0C8ABCE8-A708-420A-98BF-33B097994B24}"/>
   </bookViews>
@@ -35806,7 +35806,7 @@
   <dimension ref="A1:H28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="B5" sqref="B5:C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -35883,7 +35883,7 @@
         <v>909</v>
       </c>
       <c r="B5" s="27">
-        <v>41697</v>
+        <v>45349</v>
       </c>
       <c r="C5" s="28"/>
       <c r="D5" s="4"/>

</xml_diff>